<commit_message>
3 modul disamakan resutlnya
</commit_message>
<xml_diff>
--- a/data/template/raw data untuk crosscek pam baru.xlsx
+++ b/data/template/raw data untuk crosscek pam baru.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://icrafcifor-my.sharepoint.com/personal/d_bodro_cifor-icraf_org/Documents/dw/project R/theme 2/lusita/data/template/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://icrafcifor-my.sharepoint.com/personal/d_bodro_cifor-icraf_org/Documents/Documents/GitHub/LUSITA/data/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="166" documentId="8_{C9953028-729E-4230-BDED-2387E9D6C9CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3AE3ADE1-B9BC-402E-8629-DB01C291D862}"/>
+  <xr:revisionPtr revIDLastSave="173" documentId="8_{C9953028-729E-4230-BDED-2387E9D6C9CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{460D48CE-CABD-4BDD-90ED-6F0420A6767D}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{434F79F2-1D89-4230-B38A-FBCE8A0F0489}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{434F79F2-1D89-4230-B38A-FBCE8A0F0489}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="155">
   <si>
     <t>Urea</t>
   </si>
@@ -396,6 +396,111 @@
   </si>
   <si>
     <t>sampingan</t>
+  </si>
+  <si>
+    <t>Cengkeh Monokultur</t>
+  </si>
+  <si>
+    <t>Tahun Analisis</t>
+  </si>
+  <si>
+    <t>Tanaman Utama</t>
+  </si>
+  <si>
+    <t>Kapuk</t>
+  </si>
+  <si>
+    <t>Sistem</t>
+  </si>
+  <si>
+    <t>Agroforestry</t>
+  </si>
+  <si>
+    <t>Lokasi</t>
+  </si>
+  <si>
+    <t>Sulawesi Selatan</t>
+  </si>
+  <si>
+    <t>Luas pengelolaan</t>
+  </si>
+  <si>
+    <t>ha</t>
+  </si>
+  <si>
+    <t>Siklus Tanaman Utama</t>
+  </si>
+  <si>
+    <t>Tahun</t>
+  </si>
+  <si>
+    <t>Hasil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NPV (Rp/ha) </t>
+  </si>
+  <si>
+    <t>NPV(USD/ha)</t>
+  </si>
+  <si>
+    <t>EAE (Rp/ha)</t>
+  </si>
+  <si>
+    <t>Return to Labor (Rp/ha)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Harga Komoditas </t>
+  </si>
+  <si>
+    <t>Unit</t>
+  </si>
+  <si>
+    <t>Rp Per Unit</t>
+  </si>
+  <si>
+    <t>IRR</t>
+  </si>
+  <si>
+    <t>Gross Benefit Cost Ratio (Gross BCR)</t>
+  </si>
+  <si>
+    <t>Biaya Pembangunan/Investasi (tahun pertama saja, Rp/Ha)</t>
+  </si>
+  <si>
+    <t>Labor Cost (selama 1 siklus)</t>
+  </si>
+  <si>
+    <t>Non Labor Cost (selama 1 siklus) (Rp/Ha)</t>
+  </si>
+  <si>
+    <t>Kebutuhan TK (1tahun pertama saja, HOK/Ha)</t>
+  </si>
+  <si>
+    <t>Biaya investasi (hingga awal panen, Rp/Ha)</t>
+  </si>
+  <si>
+    <t>Kebutuhan TK (hingga awal panen, HOK/Ha)</t>
+  </si>
+  <si>
+    <t>Komoditas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jumlah Kg Bibit/Ha/musim tanam </t>
+  </si>
+  <si>
+    <t>Jarak Tanam</t>
+  </si>
+  <si>
+    <t>Profitability Index (PI)</t>
+  </si>
+  <si>
+    <t>10x10 m</t>
+  </si>
+  <si>
+    <t>15x15 m</t>
+  </si>
+  <si>
+    <t>100x20 cm</t>
   </si>
 </sst>
 </file>
@@ -813,10 +918,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E76978D-30F8-4CCF-8060-75D8D0F1ED70}">
-  <dimension ref="A1:AG187"/>
+  <dimension ref="A1:AG189"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A139" workbookViewId="0">
-      <selection activeCell="D138" sqref="D138:G138"/>
+    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
+      <selection activeCell="C124" sqref="B72:C124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -825,7 +930,10 @@
     <col min="2" max="2" width="31" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="27" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="49.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="27" width="12" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="7.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3896,7 +4004,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>36</v>
       </c>
@@ -3910,12 +4018,15 @@
         <v>1750</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F71" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>0</v>
       </c>
@@ -3925,8 +4036,14 @@
       <c r="C72">
         <v>3800</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F72" t="s">
+        <v>121</v>
+      </c>
+      <c r="G72">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>2</v>
       </c>
@@ -3936,8 +4053,14 @@
       <c r="C73">
         <v>3000</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F73" t="s">
+        <v>122</v>
+      </c>
+      <c r="G73" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>57</v>
       </c>
@@ -3947,8 +4070,14 @@
       <c r="C74">
         <v>123500</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F74" t="s">
+        <v>124</v>
+      </c>
+      <c r="G74" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>58</v>
       </c>
@@ -3958,8 +4087,14 @@
       <c r="C75">
         <v>80000</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F75" t="s">
+        <v>126</v>
+      </c>
+      <c r="G75" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>59</v>
       </c>
@@ -3969,8 +4104,17 @@
       <c r="C76">
         <v>80000</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F76" t="s">
+        <v>128</v>
+      </c>
+      <c r="G76">
+        <v>1</v>
+      </c>
+      <c r="H76" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>60</v>
       </c>
@@ -3980,8 +4124,17 @@
       <c r="C77">
         <v>1000</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F77" t="s">
+        <v>130</v>
+      </c>
+      <c r="G77">
+        <v>30</v>
+      </c>
+      <c r="H77" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>62</v>
       </c>
@@ -3992,7 +4145,7 @@
         <v>75000</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>64</v>
       </c>
@@ -4002,8 +4155,14 @@
       <c r="C79">
         <v>2000000</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F79" t="s">
+        <v>46</v>
+      </c>
+      <c r="J79" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>65</v>
       </c>
@@ -4013,8 +4172,23 @@
       <c r="C80">
         <v>125000</v>
       </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="F80" t="s">
+        <v>47</v>
+      </c>
+      <c r="G80" t="s">
+        <v>48</v>
+      </c>
+      <c r="H80">
+        <v>7.0999999999999994E-2</v>
+      </c>
+      <c r="J80" t="s">
+        <v>133</v>
+      </c>
+      <c r="K80" s="9">
+        <v>136865428.80637375</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>66</v>
       </c>
@@ -4024,8 +4198,23 @@
       <c r="C81">
         <v>105000</v>
       </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="F81" t="s">
+        <v>49</v>
+      </c>
+      <c r="G81" t="s">
+        <v>45</v>
+      </c>
+      <c r="H81">
+        <v>120000</v>
+      </c>
+      <c r="J81" t="s">
+        <v>134</v>
+      </c>
+      <c r="K81" s="9">
+        <v>8662.3689117958074</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>67</v>
       </c>
@@ -4035,8 +4224,23 @@
       <c r="C82">
         <v>600000</v>
       </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="F82" t="s">
+        <v>50</v>
+      </c>
+      <c r="G82" t="s">
+        <v>51</v>
+      </c>
+      <c r="H82">
+        <v>15800</v>
+      </c>
+      <c r="J82" t="s">
+        <v>135</v>
+      </c>
+      <c r="K82" s="9">
+        <v>11140496.274771284</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>68</v>
       </c>
@@ -4046,8 +4250,14 @@
       <c r="C83">
         <v>3000</v>
       </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J83" t="s">
+        <v>136</v>
+      </c>
+      <c r="K83" s="9">
+        <v>364689.34120879852</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>69</v>
       </c>
@@ -4057,8 +4267,23 @@
       <c r="C84">
         <v>1000</v>
       </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="F84" t="s">
+        <v>137</v>
+      </c>
+      <c r="G84" t="s">
+        <v>138</v>
+      </c>
+      <c r="H84" t="s">
+        <v>139</v>
+      </c>
+      <c r="J84" t="s">
+        <v>140</v>
+      </c>
+      <c r="K84" s="9" t="e">
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>70</v>
       </c>
@@ -4068,8 +4293,23 @@
       <c r="C85">
         <v>80000</v>
       </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="F85" t="s">
+        <v>88</v>
+      </c>
+      <c r="G85" t="s">
+        <v>112</v>
+      </c>
+      <c r="H85">
+        <v>13250</v>
+      </c>
+      <c r="J85" t="s">
+        <v>141</v>
+      </c>
+      <c r="K85" s="9">
+        <v>1.6628644115903373</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>71</v>
       </c>
@@ -4079,8 +4319,23 @@
       <c r="C86">
         <v>3000</v>
       </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="F86" t="s">
+        <v>89</v>
+      </c>
+      <c r="G86" t="s">
+        <v>112</v>
+      </c>
+      <c r="H86">
+        <v>2000</v>
+      </c>
+      <c r="J86" t="s">
+        <v>142</v>
+      </c>
+      <c r="K86" s="9">
+        <v>35520280</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>72</v>
       </c>
@@ -4090,8 +4345,23 @@
       <c r="C87">
         <v>25000</v>
       </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="F87" t="s">
+        <v>90</v>
+      </c>
+      <c r="G87" t="s">
+        <v>112</v>
+      </c>
+      <c r="H87">
+        <v>3900</v>
+      </c>
+      <c r="J87" t="s">
+        <v>143</v>
+      </c>
+      <c r="K87" s="9">
+        <v>124544640</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>73</v>
       </c>
@@ -4101,8 +4371,23 @@
       <c r="C88">
         <v>75500</v>
       </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="F88" t="s">
+        <v>91</v>
+      </c>
+      <c r="G88" t="s">
+        <v>112</v>
+      </c>
+      <c r="H88">
+        <v>120000</v>
+      </c>
+      <c r="J88" t="s">
+        <v>144</v>
+      </c>
+      <c r="K88" s="9">
+        <v>311402069</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>74</v>
       </c>
@@ -4112,8 +4397,14 @@
       <c r="C89">
         <v>115000</v>
       </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J89" t="s">
+        <v>145</v>
+      </c>
+      <c r="K89" s="9">
+        <v>165.624</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>75</v>
       </c>
@@ -4123,8 +4414,14 @@
       <c r="C90">
         <v>180000</v>
       </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J90" t="s">
+        <v>146</v>
+      </c>
+      <c r="K90" s="9">
+        <v>129923117.5</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>76</v>
       </c>
@@ -4134,8 +4431,14 @@
       <c r="C91">
         <v>25000</v>
       </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="J91" t="s">
+        <v>147</v>
+      </c>
+      <c r="K91" s="9">
+        <v>662.23199999999974</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>77</v>
       </c>
@@ -4145,8 +4448,23 @@
       <c r="C92">
         <v>3000</v>
       </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="F92" t="s">
+        <v>148</v>
+      </c>
+      <c r="G92" t="s">
+        <v>149</v>
+      </c>
+      <c r="H92" t="s">
+        <v>150</v>
+      </c>
+      <c r="J92" t="s">
+        <v>151</v>
+      </c>
+      <c r="K92" s="9">
+        <v>10.702156633259371</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>78</v>
       </c>
@@ -4156,8 +4474,17 @@
       <c r="C93">
         <v>9000000</v>
       </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="F93" t="s">
+        <v>88</v>
+      </c>
+      <c r="G93">
+        <v>63</v>
+      </c>
+      <c r="H93" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>79</v>
       </c>
@@ -4167,8 +4494,17 @@
       <c r="C94">
         <v>25000</v>
       </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="F94" t="s">
+        <v>89</v>
+      </c>
+      <c r="G94">
+        <v>28</v>
+      </c>
+      <c r="H94" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>80</v>
       </c>
@@ -4178,8 +4514,17 @@
       <c r="C95">
         <v>75000</v>
       </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="F95" t="s">
+        <v>90</v>
+      </c>
+      <c r="G95">
+        <v>20</v>
+      </c>
+      <c r="H95" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>81</v>
       </c>
@@ -4188,6 +4533,12 @@
       </c>
       <c r="C96">
         <v>4000</v>
+      </c>
+      <c r="F96" t="s">
+        <v>91</v>
+      </c>
+      <c r="G96">
+        <v>14</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.3">
@@ -4498,71 +4849,48 @@
         <v>120000</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A125" t="s">
-        <v>88</v>
-      </c>
-      <c r="B125" t="s">
-        <v>61</v>
-      </c>
-      <c r="C125">
-        <v>13250</v>
-      </c>
-    </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B126" t="s">
         <v>61</v>
       </c>
       <c r="C126">
-        <v>2000</v>
+        <v>13250</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B127" t="s">
         <v>61</v>
       </c>
       <c r="C127">
-        <v>3900</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B128" t="s">
         <v>61</v>
       </c>
       <c r="C128">
+        <v>3900</v>
+      </c>
+    </row>
+    <row r="129" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="A129" t="s">
+        <v>91</v>
+      </c>
+      <c r="B129" t="s">
+        <v>61</v>
+      </c>
+      <c r="C129">
         <v>120000</v>
-      </c>
-    </row>
-    <row r="131" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A131" t="s">
-        <v>32</v>
-      </c>
-      <c r="B131" t="s">
-        <v>0</v>
-      </c>
-      <c r="C131" t="s">
-        <v>1</v>
-      </c>
-      <c r="D131">
-        <v>400</v>
-      </c>
-      <c r="E131">
-        <v>375</v>
-      </c>
-      <c r="F131">
-        <v>325</v>
-      </c>
-      <c r="G131">
-        <v>250</v>
       </c>
     </row>
     <row r="132" spans="1:33" x14ac:dyDescent="0.3">
@@ -4570,53 +4898,53 @@
         <v>32</v>
       </c>
       <c r="B132" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C132" t="s">
         <v>1</v>
       </c>
       <c r="D132">
-        <v>320</v>
+        <v>400</v>
       </c>
       <c r="E132">
-        <v>300</v>
+        <v>375</v>
       </c>
       <c r="F132">
-        <v>260</v>
+        <v>325</v>
       </c>
       <c r="G132">
-        <v>200</v>
+        <v>250</v>
       </c>
     </row>
     <row r="133" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>116</v>
+        <v>32</v>
       </c>
       <c r="B133" t="s">
-        <v>57</v>
+        <v>2</v>
       </c>
       <c r="C133" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="D133">
-        <v>1.6</v>
+        <v>320</v>
       </c>
       <c r="E133">
-        <v>1.5</v>
+        <v>300</v>
       </c>
       <c r="F133">
-        <v>1.3</v>
+        <v>260</v>
       </c>
       <c r="G133">
-        <v>1</v>
+        <v>200</v>
       </c>
     </row>
     <row r="134" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B134" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C134" t="s">
         <v>8</v>
@@ -4636,273 +4964,195 @@
     </row>
     <row r="135" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B135" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C135" t="s">
         <v>8</v>
       </c>
       <c r="D135">
-        <v>3.2</v>
+        <v>1.6</v>
       </c>
       <c r="E135">
-        <v>3</v>
+        <v>1.5</v>
       </c>
       <c r="F135">
-        <v>2.6</v>
+        <v>1.3</v>
       </c>
       <c r="G135">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="136" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>32</v>
+        <v>117</v>
       </c>
       <c r="B136" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C136" t="s">
-        <v>112</v>
+        <v>8</v>
       </c>
       <c r="D136">
-        <v>1600</v>
+        <v>3.2</v>
       </c>
       <c r="E136">
-        <v>1500</v>
+        <v>3</v>
       </c>
       <c r="F136">
-        <v>1300</v>
+        <v>2.6</v>
       </c>
       <c r="G136">
-        <v>1000</v>
+        <v>2</v>
       </c>
     </row>
     <row r="137" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>116</v>
+        <v>32</v>
       </c>
       <c r="B137" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C137" t="s">
-        <v>8</v>
+        <v>112</v>
       </c>
       <c r="D137">
-        <v>3.2</v>
+        <v>1600</v>
       </c>
       <c r="E137">
-        <v>3</v>
+        <v>1500</v>
       </c>
       <c r="F137">
-        <v>2.6</v>
+        <v>1300</v>
       </c>
       <c r="G137">
-        <v>2</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="138" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>32</v>
+        <v>116</v>
       </c>
       <c r="B138" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C138" t="s">
-        <v>113</v>
+        <v>8</v>
       </c>
       <c r="D138">
-        <v>0</v>
+        <v>3.2</v>
       </c>
       <c r="E138">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F138">
-        <v>0</v>
+        <v>2.6</v>
       </c>
       <c r="G138">
-        <v>0</v>
-      </c>
-      <c r="H138">
-        <v>1</v>
-      </c>
-      <c r="I138">
-        <v>1</v>
-      </c>
-      <c r="J138">
-        <v>1</v>
-      </c>
-      <c r="K138">
-        <v>1</v>
-      </c>
-      <c r="L138">
-        <v>1</v>
-      </c>
-      <c r="M138">
-        <v>1</v>
-      </c>
-      <c r="N138">
-        <v>1</v>
-      </c>
-      <c r="O138">
-        <v>1</v>
-      </c>
-      <c r="P138">
-        <v>1</v>
-      </c>
-      <c r="Q138">
-        <v>1</v>
-      </c>
-      <c r="R138">
-        <v>1</v>
-      </c>
-      <c r="S138">
-        <v>1</v>
-      </c>
-      <c r="T138">
-        <v>1</v>
-      </c>
-      <c r="U138">
-        <v>1</v>
-      </c>
-      <c r="V138">
-        <v>1</v>
-      </c>
-      <c r="W138">
-        <v>1</v>
-      </c>
-      <c r="X138">
-        <v>1</v>
-      </c>
-      <c r="Y138">
-        <v>1</v>
-      </c>
-      <c r="Z138">
-        <v>1</v>
-      </c>
-      <c r="AA138">
-        <v>1</v>
-      </c>
-      <c r="AB138">
-        <v>1</v>
-      </c>
-      <c r="AC138">
-        <v>1</v>
-      </c>
-      <c r="AD138">
-        <v>1</v>
-      </c>
-      <c r="AE138">
-        <v>1</v>
-      </c>
-      <c r="AF138">
-        <v>1</v>
-      </c>
-      <c r="AG138">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="139" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B139" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C139" t="s">
-        <v>11</v>
+        <v>113</v>
       </c>
       <c r="D139">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E139">
         <v>0</v>
       </c>
       <c r="F139">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G139">
         <v>0</v>
       </c>
       <c r="H139">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I139">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J139">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K139">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L139">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M139">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N139">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O139">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P139">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q139">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R139">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S139">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T139">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U139">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V139">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="W139">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X139">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Y139">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z139">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AA139">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB139">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AC139">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD139">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AE139">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF139">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AG139">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="140" spans="1:33" x14ac:dyDescent="0.3">
@@ -4910,7 +5160,7 @@
         <v>33</v>
       </c>
       <c r="B140" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C140" t="s">
         <v>11</v>
@@ -4922,25 +5172,25 @@
         <v>0</v>
       </c>
       <c r="F140">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G140">
         <v>0</v>
       </c>
       <c r="H140">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I140">
+        <v>0</v>
+      </c>
+      <c r="J140">
         <v>2</v>
       </c>
-      <c r="J140">
-        <v>0</v>
-      </c>
       <c r="K140">
         <v>0</v>
       </c>
       <c r="L140">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M140">
         <v>0</v>
@@ -4952,25 +5202,25 @@
         <v>0</v>
       </c>
       <c r="P140">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q140">
         <v>0</v>
       </c>
       <c r="R140">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="S140">
+        <v>0</v>
+      </c>
+      <c r="T140">
         <v>2</v>
       </c>
-      <c r="T140">
-        <v>0</v>
-      </c>
       <c r="U140">
         <v>0</v>
       </c>
       <c r="V140">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="W140">
         <v>0</v>
@@ -4982,25 +5232,25 @@
         <v>0</v>
       </c>
       <c r="Z140">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AA140">
         <v>0</v>
       </c>
       <c r="AB140">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AC140">
+        <v>0</v>
+      </c>
+      <c r="AD140">
         <v>2</v>
       </c>
-      <c r="AD140">
-        <v>0</v>
-      </c>
       <c r="AE140">
         <v>0</v>
       </c>
       <c r="AF140">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AG140">
         <v>0</v>
@@ -5011,7 +5261,7 @@
         <v>33</v>
       </c>
       <c r="B141" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C141" t="s">
         <v>11</v>
@@ -5112,13 +5362,13 @@
         <v>33</v>
       </c>
       <c r="B142" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C142" t="s">
         <v>11</v>
       </c>
       <c r="D142">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E142">
         <v>0</v>
@@ -5130,82 +5380,82 @@
         <v>0</v>
       </c>
       <c r="H142">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="I142">
-        <v>46</v>
+        <v>2</v>
       </c>
       <c r="J142">
-        <v>46</v>
+        <v>0</v>
       </c>
       <c r="K142">
-        <v>46</v>
+        <v>0</v>
       </c>
       <c r="L142">
-        <v>62</v>
+        <v>0</v>
       </c>
       <c r="M142">
-        <v>62</v>
+        <v>0</v>
       </c>
       <c r="N142">
-        <v>62</v>
+        <v>2</v>
       </c>
       <c r="O142">
-        <v>62</v>
+        <v>0</v>
       </c>
       <c r="P142">
-        <v>73</v>
+        <v>0</v>
       </c>
       <c r="Q142">
-        <v>73</v>
+        <v>0</v>
       </c>
       <c r="R142">
-        <v>84</v>
+        <v>0</v>
       </c>
       <c r="S142">
-        <v>84</v>
+        <v>2</v>
       </c>
       <c r="T142">
-        <v>84</v>
+        <v>0</v>
       </c>
       <c r="U142">
-        <v>84</v>
+        <v>0</v>
       </c>
       <c r="V142">
-        <v>84</v>
+        <v>0</v>
       </c>
       <c r="W142">
-        <v>84</v>
+        <v>0</v>
       </c>
       <c r="X142">
-        <v>85</v>
+        <v>2</v>
       </c>
       <c r="Y142">
-        <v>85</v>
+        <v>0</v>
       </c>
       <c r="Z142">
-        <v>85</v>
+        <v>0</v>
       </c>
       <c r="AA142">
-        <v>85</v>
+        <v>0</v>
       </c>
       <c r="AB142">
-        <v>85</v>
+        <v>0</v>
       </c>
       <c r="AC142">
-        <v>85</v>
+        <v>2</v>
       </c>
       <c r="AD142">
-        <v>85</v>
+        <v>0</v>
       </c>
       <c r="AE142">
-        <v>85</v>
+        <v>0</v>
       </c>
       <c r="AF142">
-        <v>85</v>
+        <v>0</v>
       </c>
       <c r="AG142">
-        <v>85</v>
+        <v>0</v>
       </c>
     </row>
     <row r="143" spans="1:33" x14ac:dyDescent="0.3">
@@ -5213,16 +5463,16 @@
         <v>33</v>
       </c>
       <c r="B143" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C143" t="s">
         <v>11</v>
       </c>
       <c r="D143">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="E143">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F143">
         <v>0</v>
@@ -5231,82 +5481,82 @@
         <v>0</v>
       </c>
       <c r="H143">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="I143">
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="J143">
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="K143">
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="L143">
-        <v>0</v>
+        <v>62</v>
       </c>
       <c r="M143">
-        <v>0</v>
+        <v>62</v>
       </c>
       <c r="N143">
-        <v>0</v>
+        <v>62</v>
       </c>
       <c r="O143">
-        <v>0</v>
+        <v>62</v>
       </c>
       <c r="P143">
-        <v>0</v>
+        <v>73</v>
       </c>
       <c r="Q143">
-        <v>0</v>
+        <v>73</v>
       </c>
       <c r="R143">
-        <v>0</v>
+        <v>84</v>
       </c>
       <c r="S143">
-        <v>0</v>
+        <v>84</v>
       </c>
       <c r="T143">
-        <v>0</v>
+        <v>84</v>
       </c>
       <c r="U143">
-        <v>0</v>
+        <v>84</v>
       </c>
       <c r="V143">
-        <v>0</v>
+        <v>84</v>
       </c>
       <c r="W143">
-        <v>0</v>
+        <v>84</v>
       </c>
       <c r="X143">
-        <v>0</v>
+        <v>85</v>
       </c>
       <c r="Y143">
-        <v>0</v>
+        <v>85</v>
       </c>
       <c r="Z143">
-        <v>0</v>
+        <v>85</v>
       </c>
       <c r="AA143">
-        <v>0</v>
+        <v>85</v>
       </c>
       <c r="AB143">
-        <v>0</v>
+        <v>85</v>
       </c>
       <c r="AC143">
-        <v>0</v>
+        <v>85</v>
       </c>
       <c r="AD143">
-        <v>0</v>
+        <v>85</v>
       </c>
       <c r="AE143">
-        <v>0</v>
+        <v>85</v>
       </c>
       <c r="AF143">
-        <v>0</v>
+        <v>85</v>
       </c>
       <c r="AG143">
-        <v>0</v>
+        <v>85</v>
       </c>
     </row>
     <row r="144" spans="1:33" x14ac:dyDescent="0.3">
@@ -5314,16 +5564,16 @@
         <v>33</v>
       </c>
       <c r="B144" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C144" t="s">
         <v>11</v>
       </c>
       <c r="D144">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="E144">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F144">
         <v>0</v>
@@ -5335,7 +5585,7 @@
         <v>0</v>
       </c>
       <c r="I144">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J144">
         <v>0</v>
@@ -5350,7 +5600,7 @@
         <v>0</v>
       </c>
       <c r="N144">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O144">
         <v>0</v>
@@ -5365,7 +5615,7 @@
         <v>0</v>
       </c>
       <c r="S144">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T144">
         <v>0</v>
@@ -5380,7 +5630,7 @@
         <v>0</v>
       </c>
       <c r="X144">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y144">
         <v>0</v>
@@ -5395,7 +5645,7 @@
         <v>0</v>
       </c>
       <c r="AC144">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD144">
         <v>0</v>
@@ -5415,13 +5665,13 @@
         <v>33</v>
       </c>
       <c r="B145" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C145" t="s">
         <v>11</v>
       </c>
       <c r="D145">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E145">
         <v>0</v>
@@ -5430,85 +5680,85 @@
         <v>0</v>
       </c>
       <c r="G145">
-        <v>1.89</v>
+        <v>0</v>
       </c>
       <c r="H145">
-        <v>2.3624999999999998</v>
+        <v>0</v>
       </c>
       <c r="I145">
-        <v>2.835</v>
+        <v>1</v>
       </c>
       <c r="J145">
-        <v>3.3075000000000001</v>
+        <v>0</v>
       </c>
       <c r="K145">
-        <v>3.78</v>
+        <v>0</v>
       </c>
       <c r="L145">
-        <v>4.2525000000000004</v>
+        <v>0</v>
       </c>
       <c r="M145">
-        <v>4.7249999999999996</v>
+        <v>0</v>
       </c>
       <c r="N145">
-        <v>5.1974999999999998</v>
+        <v>1</v>
       </c>
       <c r="O145">
-        <v>6.1425000000000001</v>
+        <v>0</v>
       </c>
       <c r="P145">
-        <v>7.0875000000000004</v>
+        <v>0</v>
       </c>
       <c r="Q145">
-        <v>8.0325000000000006</v>
+        <v>0</v>
       </c>
       <c r="R145">
-        <v>8.9774999999999991</v>
+        <v>0</v>
       </c>
       <c r="S145">
-        <v>9.9224999999999994</v>
+        <v>1</v>
       </c>
       <c r="T145">
-        <v>10.8675</v>
+        <v>0</v>
       </c>
       <c r="U145">
-        <v>10.395</v>
+        <v>0</v>
       </c>
       <c r="V145">
-        <v>9.9224999999999994</v>
+        <v>0</v>
       </c>
       <c r="W145">
-        <v>9.4499999999999993</v>
+        <v>0</v>
       </c>
       <c r="X145">
-        <v>8.9774999999999991</v>
+        <v>1</v>
       </c>
       <c r="Y145">
-        <v>8.5050000000000008</v>
+        <v>0</v>
       </c>
       <c r="Z145">
-        <v>8.0325000000000006</v>
+        <v>0</v>
       </c>
       <c r="AA145">
-        <v>7.2765000000000013</v>
+        <v>0</v>
       </c>
       <c r="AB145">
-        <v>6.5205000000000011</v>
+        <v>0</v>
       </c>
       <c r="AC145">
-        <v>5.7645000000000008</v>
+        <v>1</v>
       </c>
       <c r="AD145">
-        <v>5.0085000000000006</v>
+        <v>0</v>
       </c>
       <c r="AE145">
-        <v>4.5360000000000005</v>
+        <v>0</v>
       </c>
       <c r="AF145">
-        <v>4.0635000000000012</v>
+        <v>0</v>
       </c>
       <c r="AG145">
-        <v>3.5910000000000006</v>
+        <v>0</v>
       </c>
     </row>
     <row r="146" spans="1:33" x14ac:dyDescent="0.3">
@@ -5516,13 +5766,13 @@
         <v>33</v>
       </c>
       <c r="B146" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C146" t="s">
         <v>11</v>
       </c>
       <c r="D146">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E146">
         <v>0</v>
@@ -5531,85 +5781,85 @@
         <v>0</v>
       </c>
       <c r="G146">
-        <v>0</v>
+        <v>1.89</v>
       </c>
       <c r="H146">
-        <v>0</v>
+        <v>2.3624999999999998</v>
       </c>
       <c r="I146">
-        <v>1</v>
+        <v>2.835</v>
       </c>
       <c r="J146">
-        <v>0</v>
+        <v>3.3075000000000001</v>
       </c>
       <c r="K146">
-        <v>0</v>
+        <v>3.78</v>
       </c>
       <c r="L146">
-        <v>0</v>
+        <v>4.2525000000000004</v>
       </c>
       <c r="M146">
-        <v>0</v>
+        <v>4.7249999999999996</v>
       </c>
       <c r="N146">
-        <v>1</v>
+        <v>5.1974999999999998</v>
       </c>
       <c r="O146">
-        <v>0</v>
+        <v>6.1425000000000001</v>
       </c>
       <c r="P146">
-        <v>0</v>
+        <v>7.0875000000000004</v>
       </c>
       <c r="Q146">
-        <v>0</v>
+        <v>8.0325000000000006</v>
       </c>
       <c r="R146">
-        <v>0</v>
+        <v>8.9774999999999991</v>
       </c>
       <c r="S146">
-        <v>1</v>
+        <v>9.9224999999999994</v>
       </c>
       <c r="T146">
-        <v>0</v>
+        <v>10.8675</v>
       </c>
       <c r="U146">
-        <v>0</v>
+        <v>10.395</v>
       </c>
       <c r="V146">
-        <v>0</v>
+        <v>9.9224999999999994</v>
       </c>
       <c r="W146">
-        <v>0</v>
+        <v>9.4499999999999993</v>
       </c>
       <c r="X146">
-        <v>1</v>
+        <v>8.9774999999999991</v>
       </c>
       <c r="Y146">
-        <v>0</v>
+        <v>8.5050000000000008</v>
       </c>
       <c r="Z146">
-        <v>0</v>
+        <v>8.0325000000000006</v>
       </c>
       <c r="AA146">
-        <v>0</v>
+        <v>7.2765000000000013</v>
       </c>
       <c r="AB146">
-        <v>0</v>
+        <v>6.5205000000000011</v>
       </c>
       <c r="AC146">
-        <v>1</v>
+        <v>5.7645000000000008</v>
       </c>
       <c r="AD146">
-        <v>0</v>
+        <v>5.0085000000000006</v>
       </c>
       <c r="AE146">
-        <v>0</v>
+        <v>4.5360000000000005</v>
       </c>
       <c r="AF146">
-        <v>0</v>
+        <v>4.0635000000000012</v>
       </c>
       <c r="AG146">
-        <v>0</v>
+        <v>3.5910000000000006</v>
       </c>
     </row>
     <row r="147" spans="1:33" x14ac:dyDescent="0.3">
@@ -5617,13 +5867,13 @@
         <v>33</v>
       </c>
       <c r="B147" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C147" t="s">
         <v>11</v>
       </c>
       <c r="D147">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E147">
         <v>0</v>
@@ -5638,7 +5888,7 @@
         <v>0</v>
       </c>
       <c r="I147">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J147">
         <v>0</v>
@@ -5653,7 +5903,7 @@
         <v>0</v>
       </c>
       <c r="N147">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O147">
         <v>0</v>
@@ -5668,7 +5918,7 @@
         <v>0</v>
       </c>
       <c r="S147">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T147">
         <v>0</v>
@@ -5683,7 +5933,7 @@
         <v>0</v>
       </c>
       <c r="X147">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y147">
         <v>0</v>
@@ -5698,7 +5948,7 @@
         <v>0</v>
       </c>
       <c r="AC147">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD147">
         <v>0</v>
@@ -5718,7 +5968,7 @@
         <v>33</v>
       </c>
       <c r="B148" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C148" t="s">
         <v>11</v>
@@ -5819,13 +6069,13 @@
         <v>33</v>
       </c>
       <c r="B149" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C149" t="s">
         <v>11</v>
       </c>
       <c r="D149">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="E149">
         <v>0</v>
@@ -5920,13 +6170,13 @@
         <v>33</v>
       </c>
       <c r="B150" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C150" t="s">
         <v>11</v>
       </c>
       <c r="D150">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="E150">
         <v>0</v>
@@ -6021,22 +6271,22 @@
         <v>33</v>
       </c>
       <c r="B151" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C151" t="s">
         <v>11</v>
       </c>
       <c r="D151">
-        <v>201.6</v>
+        <v>2</v>
       </c>
       <c r="E151">
-        <v>189</v>
+        <v>0</v>
       </c>
       <c r="F151">
-        <v>163.80000000000001</v>
+        <v>0</v>
       </c>
       <c r="G151">
-        <v>126</v>
+        <v>0</v>
       </c>
       <c r="H151">
         <v>0</v>
@@ -6122,25 +6372,25 @@
         <v>33</v>
       </c>
       <c r="B152" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C152" t="s">
         <v>11</v>
       </c>
       <c r="D152">
-        <v>0</v>
+        <v>201.6</v>
       </c>
       <c r="E152">
-        <v>0</v>
+        <v>189</v>
       </c>
       <c r="F152">
-        <v>0</v>
+        <v>163.80000000000001</v>
       </c>
       <c r="G152">
-        <v>0</v>
+        <v>126</v>
       </c>
       <c r="H152">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I152">
         <v>0</v>
@@ -6155,7 +6405,7 @@
         <v>0</v>
       </c>
       <c r="M152">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N152">
         <v>0</v>
@@ -6170,7 +6420,7 @@
         <v>0</v>
       </c>
       <c r="R152">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S152">
         <v>0</v>
@@ -6185,7 +6435,7 @@
         <v>0</v>
       </c>
       <c r="W152">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X152">
         <v>0</v>
@@ -6200,7 +6450,7 @@
         <v>0</v>
       </c>
       <c r="AB152">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC152">
         <v>0</v>
@@ -6215,7 +6465,7 @@
         <v>0</v>
       </c>
       <c r="AG152">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="153" spans="1:33" x14ac:dyDescent="0.3">
@@ -6223,7 +6473,7 @@
         <v>33</v>
       </c>
       <c r="B153" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C153" t="s">
         <v>11</v>
@@ -6241,82 +6491,82 @@
         <v>0</v>
       </c>
       <c r="H153">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I153">
         <v>0</v>
       </c>
       <c r="J153">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K153">
         <v>0</v>
       </c>
       <c r="L153">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M153">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N153">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O153">
         <v>0</v>
       </c>
       <c r="P153">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Q153">
         <v>0</v>
       </c>
       <c r="R153">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S153">
         <v>0</v>
       </c>
       <c r="T153">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="U153">
         <v>0</v>
       </c>
       <c r="V153">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="W153">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X153">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Y153">
         <v>0</v>
       </c>
       <c r="Z153">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AA153">
         <v>0</v>
       </c>
       <c r="AB153">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AC153">
         <v>0</v>
       </c>
       <c r="AD153">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AE153">
         <v>0</v>
       </c>
       <c r="AF153">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AG153">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="154" spans="1:33" x14ac:dyDescent="0.3">
@@ -6324,7 +6574,7 @@
         <v>33</v>
       </c>
       <c r="B154" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C154" t="s">
         <v>11</v>
@@ -6342,82 +6592,82 @@
         <v>0</v>
       </c>
       <c r="H154">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="I154">
         <v>0</v>
       </c>
       <c r="J154">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K154">
         <v>0</v>
       </c>
       <c r="L154">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M154">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="N154">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O154">
         <v>0</v>
       </c>
       <c r="P154">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q154">
         <v>0</v>
       </c>
       <c r="R154">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="S154">
         <v>0</v>
       </c>
       <c r="T154">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="U154">
         <v>0</v>
       </c>
       <c r="V154">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="W154">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="X154">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Y154">
         <v>0</v>
       </c>
       <c r="Z154">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AA154">
         <v>0</v>
       </c>
       <c r="AB154">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="AC154">
         <v>0</v>
       </c>
       <c r="AD154">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AE154">
         <v>0</v>
       </c>
       <c r="AF154">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AG154">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="155" spans="1:33" x14ac:dyDescent="0.3">
@@ -6425,7 +6675,7 @@
         <v>33</v>
       </c>
       <c r="B155" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C155" t="s">
         <v>11</v>
@@ -6443,82 +6693,82 @@
         <v>0</v>
       </c>
       <c r="H155">
-        <v>672</v>
+        <v>5</v>
       </c>
       <c r="I155">
-        <v>672</v>
+        <v>0</v>
       </c>
       <c r="J155">
-        <v>672</v>
+        <v>0</v>
       </c>
       <c r="K155">
-        <v>672</v>
+        <v>0</v>
       </c>
       <c r="L155">
-        <v>672</v>
+        <v>0</v>
       </c>
       <c r="M155">
-        <v>672</v>
+        <v>5</v>
       </c>
       <c r="N155">
-        <v>672</v>
+        <v>0</v>
       </c>
       <c r="O155">
-        <v>672</v>
+        <v>0</v>
       </c>
       <c r="P155">
-        <v>672</v>
+        <v>0</v>
       </c>
       <c r="Q155">
-        <v>672</v>
+        <v>0</v>
       </c>
       <c r="R155">
-        <v>672</v>
+        <v>5</v>
       </c>
       <c r="S155">
-        <v>672</v>
+        <v>0</v>
       </c>
       <c r="T155">
-        <v>672</v>
+        <v>0</v>
       </c>
       <c r="U155">
-        <v>672</v>
+        <v>0</v>
       </c>
       <c r="V155">
-        <v>672</v>
+        <v>0</v>
       </c>
       <c r="W155">
-        <v>672</v>
+        <v>5</v>
       </c>
       <c r="X155">
-        <v>672</v>
+        <v>0</v>
       </c>
       <c r="Y155">
-        <v>672</v>
+        <v>0</v>
       </c>
       <c r="Z155">
-        <v>672</v>
+        <v>0</v>
       </c>
       <c r="AA155">
-        <v>672</v>
+        <v>0</v>
       </c>
       <c r="AB155">
-        <v>672</v>
+        <v>5</v>
       </c>
       <c r="AC155">
-        <v>672</v>
+        <v>0</v>
       </c>
       <c r="AD155">
-        <v>672</v>
+        <v>0</v>
       </c>
       <c r="AE155">
-        <v>672</v>
+        <v>0</v>
       </c>
       <c r="AF155">
-        <v>672</v>
+        <v>0</v>
       </c>
       <c r="AG155">
-        <v>672</v>
+        <v>5</v>
       </c>
     </row>
     <row r="156" spans="1:33" x14ac:dyDescent="0.3">
@@ -6526,7 +6776,7 @@
         <v>33</v>
       </c>
       <c r="B156" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C156" t="s">
         <v>11</v>
@@ -6544,82 +6794,82 @@
         <v>0</v>
       </c>
       <c r="H156">
-        <v>2</v>
+        <v>672</v>
       </c>
       <c r="I156">
-        <v>0</v>
+        <v>672</v>
       </c>
       <c r="J156">
-        <v>2</v>
+        <v>672</v>
       </c>
       <c r="K156">
-        <v>0</v>
+        <v>672</v>
       </c>
       <c r="L156">
-        <v>2</v>
+        <v>672</v>
       </c>
       <c r="M156">
-        <v>0</v>
+        <v>672</v>
       </c>
       <c r="N156">
-        <v>2</v>
+        <v>672</v>
       </c>
       <c r="O156">
-        <v>0</v>
+        <v>672</v>
       </c>
       <c r="P156">
-        <v>2</v>
+        <v>672</v>
       </c>
       <c r="Q156">
-        <v>0</v>
+        <v>672</v>
       </c>
       <c r="R156">
-        <v>2</v>
+        <v>672</v>
       </c>
       <c r="S156">
-        <v>0</v>
+        <v>672</v>
       </c>
       <c r="T156">
-        <v>2</v>
+        <v>672</v>
       </c>
       <c r="U156">
-        <v>0</v>
+        <v>672</v>
       </c>
       <c r="V156">
-        <v>2</v>
+        <v>672</v>
       </c>
       <c r="W156">
-        <v>0</v>
+        <v>672</v>
       </c>
       <c r="X156">
-        <v>2</v>
+        <v>672</v>
       </c>
       <c r="Y156">
-        <v>0</v>
+        <v>672</v>
       </c>
       <c r="Z156">
-        <v>2</v>
+        <v>672</v>
       </c>
       <c r="AA156">
-        <v>0</v>
+        <v>672</v>
       </c>
       <c r="AB156">
-        <v>2</v>
+        <v>672</v>
       </c>
       <c r="AC156">
-        <v>0</v>
+        <v>672</v>
       </c>
       <c r="AD156">
-        <v>2</v>
+        <v>672</v>
       </c>
       <c r="AE156">
-        <v>0</v>
+        <v>672</v>
       </c>
       <c r="AF156">
-        <v>2</v>
+        <v>672</v>
       </c>
       <c r="AG156">
-        <v>0</v>
+        <v>672</v>
       </c>
     </row>
     <row r="157" spans="1:33" x14ac:dyDescent="0.3">
@@ -6627,7 +6877,7 @@
         <v>33</v>
       </c>
       <c r="B157" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C157" t="s">
         <v>11</v>
@@ -6728,7 +6978,7 @@
         <v>33</v>
       </c>
       <c r="B158" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C158" t="s">
         <v>11</v>
@@ -6829,7 +7079,7 @@
         <v>33</v>
       </c>
       <c r="B159" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C159" t="s">
         <v>11</v>
@@ -6844,82 +7094,82 @@
         <v>0</v>
       </c>
       <c r="G159">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="H159">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I159">
         <v>0</v>
       </c>
       <c r="J159">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K159">
         <v>0</v>
       </c>
       <c r="L159">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="M159">
         <v>0</v>
       </c>
       <c r="N159">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O159">
         <v>0</v>
       </c>
       <c r="P159">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q159">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="R159">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="S159">
         <v>0</v>
       </c>
       <c r="T159">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="U159">
         <v>0</v>
       </c>
       <c r="V159">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="W159">
         <v>0</v>
       </c>
       <c r="X159">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Y159">
         <v>0</v>
       </c>
       <c r="Z159">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AA159">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="AB159">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AC159">
         <v>0</v>
       </c>
       <c r="AD159">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AE159">
         <v>0</v>
       </c>
       <c r="AF159">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AG159">
         <v>0</v>
@@ -6927,19 +7177,103 @@
     </row>
     <row r="160" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B160" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C160" t="s">
-        <v>114</v>
+        <v>11</v>
       </c>
       <c r="D160">
-        <v>63</v>
+        <v>0</v>
       </c>
       <c r="E160">
-        <v>6.3000000000000007</v>
+        <v>0</v>
+      </c>
+      <c r="F160">
+        <v>0</v>
+      </c>
+      <c r="G160">
+        <v>14</v>
+      </c>
+      <c r="H160">
+        <v>0</v>
+      </c>
+      <c r="I160">
+        <v>0</v>
+      </c>
+      <c r="J160">
+        <v>0</v>
+      </c>
+      <c r="K160">
+        <v>0</v>
+      </c>
+      <c r="L160">
+        <v>14</v>
+      </c>
+      <c r="M160">
+        <v>0</v>
+      </c>
+      <c r="N160">
+        <v>0</v>
+      </c>
+      <c r="O160">
+        <v>0</v>
+      </c>
+      <c r="P160">
+        <v>0</v>
+      </c>
+      <c r="Q160">
+        <v>14</v>
+      </c>
+      <c r="R160">
+        <v>0</v>
+      </c>
+      <c r="S160">
+        <v>0</v>
+      </c>
+      <c r="T160">
+        <v>0</v>
+      </c>
+      <c r="U160">
+        <v>0</v>
+      </c>
+      <c r="V160">
+        <v>14</v>
+      </c>
+      <c r="W160">
+        <v>0</v>
+      </c>
+      <c r="X160">
+        <v>0</v>
+      </c>
+      <c r="Y160">
+        <v>0</v>
+      </c>
+      <c r="Z160">
+        <v>0</v>
+      </c>
+      <c r="AA160">
+        <v>14</v>
+      </c>
+      <c r="AB160">
+        <v>0</v>
+      </c>
+      <c r="AC160">
+        <v>0</v>
+      </c>
+      <c r="AD160">
+        <v>0</v>
+      </c>
+      <c r="AE160">
+        <v>0</v>
+      </c>
+      <c r="AF160">
+        <v>0</v>
+      </c>
+      <c r="AG160">
+        <v>0</v>
       </c>
     </row>
     <row r="161" spans="1:33" x14ac:dyDescent="0.3">
@@ -6947,16 +7281,16 @@
         <v>34</v>
       </c>
       <c r="B161" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C161" t="s">
         <v>114</v>
       </c>
       <c r="D161">
-        <v>28</v>
+        <v>63</v>
       </c>
       <c r="E161">
-        <v>2.8000000000000003</v>
+        <v>6.3000000000000007</v>
       </c>
     </row>
     <row r="162" spans="1:33" x14ac:dyDescent="0.3">
@@ -6964,22 +7298,16 @@
         <v>34</v>
       </c>
       <c r="B162" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C162" t="s">
-        <v>1</v>
+        <v>114</v>
       </c>
       <c r="D162">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="E162">
-        <v>30</v>
-      </c>
-      <c r="F162">
-        <v>26</v>
-      </c>
-      <c r="G162">
-        <v>20</v>
+        <v>2.8000000000000003</v>
       </c>
     </row>
     <row r="163" spans="1:33" x14ac:dyDescent="0.3">
@@ -6987,114 +7315,36 @@
         <v>34</v>
       </c>
       <c r="B163" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C163" t="s">
-        <v>115</v>
+        <v>1</v>
+      </c>
+      <c r="D163">
+        <v>32</v>
+      </c>
+      <c r="E163">
+        <v>30</v>
+      </c>
+      <c r="F163">
+        <v>26</v>
       </c>
       <c r="G163">
-        <v>14</v>
+        <v>20</v>
       </c>
     </row>
     <row r="164" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B164" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C164" t="s">
-        <v>24</v>
-      </c>
-      <c r="D164">
-        <v>60</v>
-      </c>
-      <c r="E164">
-        <v>0</v>
-      </c>
-      <c r="F164">
-        <v>0</v>
+        <v>115</v>
       </c>
       <c r="G164">
-        <v>0</v>
-      </c>
-      <c r="H164">
-        <v>0</v>
-      </c>
-      <c r="I164">
-        <v>0</v>
-      </c>
-      <c r="J164">
-        <v>0</v>
-      </c>
-      <c r="K164">
-        <v>0</v>
-      </c>
-      <c r="L164">
-        <v>0</v>
-      </c>
-      <c r="M164">
-        <v>0</v>
-      </c>
-      <c r="N164">
-        <v>0</v>
-      </c>
-      <c r="O164">
-        <v>0</v>
-      </c>
-      <c r="P164">
-        <v>0</v>
-      </c>
-      <c r="Q164">
-        <v>0</v>
-      </c>
-      <c r="R164">
-        <v>0</v>
-      </c>
-      <c r="S164">
-        <v>0</v>
-      </c>
-      <c r="T164">
-        <v>0</v>
-      </c>
-      <c r="U164">
-        <v>0</v>
-      </c>
-      <c r="V164">
-        <v>0</v>
-      </c>
-      <c r="W164">
-        <v>0</v>
-      </c>
-      <c r="X164">
-        <v>0</v>
-      </c>
-      <c r="Y164">
-        <v>0</v>
-      </c>
-      <c r="Z164">
-        <v>0</v>
-      </c>
-      <c r="AA164">
-        <v>0</v>
-      </c>
-      <c r="AB164">
-        <v>0</v>
-      </c>
-      <c r="AC164">
-        <v>0</v>
-      </c>
-      <c r="AD164">
-        <v>0</v>
-      </c>
-      <c r="AE164">
-        <v>0</v>
-      </c>
-      <c r="AF164">
-        <v>0</v>
-      </c>
-      <c r="AG164">
-        <v>0</v>
+        <v>14</v>
       </c>
     </row>
     <row r="165" spans="1:33" x14ac:dyDescent="0.3">
@@ -7102,16 +7352,16 @@
         <v>35</v>
       </c>
       <c r="B165" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C165" t="s">
         <v>24</v>
       </c>
       <c r="D165">
-        <v>1.68</v>
+        <v>60</v>
       </c>
       <c r="E165">
-        <v>0.16800000000000001</v>
+        <v>0</v>
       </c>
       <c r="F165">
         <v>0</v>
@@ -7203,100 +7453,100 @@
         <v>35</v>
       </c>
       <c r="B166" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C166" t="s">
         <v>24</v>
       </c>
       <c r="D166">
-        <v>0</v>
+        <v>1.68</v>
       </c>
       <c r="E166">
-        <v>0</v>
+        <v>0.16800000000000001</v>
       </c>
       <c r="F166">
         <v>0</v>
       </c>
       <c r="G166">
-        <v>0.98000000000000009</v>
+        <v>0</v>
       </c>
       <c r="H166">
-        <v>0.98000000000000009</v>
+        <v>0</v>
       </c>
       <c r="I166">
-        <v>0.98000000000000009</v>
+        <v>0</v>
       </c>
       <c r="J166">
-        <v>0.98000000000000009</v>
+        <v>0</v>
       </c>
       <c r="K166">
-        <v>0.98000000000000009</v>
+        <v>0</v>
       </c>
       <c r="L166">
-        <v>0.98000000000000009</v>
+        <v>0</v>
       </c>
       <c r="M166">
-        <v>0.98000000000000009</v>
+        <v>0</v>
       </c>
       <c r="N166">
-        <v>0.98000000000000009</v>
+        <v>0</v>
       </c>
       <c r="O166">
-        <v>0.98000000000000009</v>
+        <v>0</v>
       </c>
       <c r="P166">
-        <v>0.98000000000000009</v>
+        <v>0</v>
       </c>
       <c r="Q166">
-        <v>0.98000000000000009</v>
+        <v>0</v>
       </c>
       <c r="R166">
-        <v>0.98000000000000009</v>
+        <v>0</v>
       </c>
       <c r="S166">
-        <v>0.98000000000000009</v>
+        <v>0</v>
       </c>
       <c r="T166">
-        <v>0.98000000000000009</v>
+        <v>0</v>
       </c>
       <c r="U166">
-        <v>0.98000000000000009</v>
+        <v>0</v>
       </c>
       <c r="V166">
-        <v>0.98000000000000009</v>
+        <v>0</v>
       </c>
       <c r="W166">
-        <v>0.98000000000000009</v>
+        <v>0</v>
       </c>
       <c r="X166">
-        <v>0.98000000000000009</v>
+        <v>0</v>
       </c>
       <c r="Y166">
-        <v>0.98000000000000009</v>
+        <v>0</v>
       </c>
       <c r="Z166">
-        <v>0.98000000000000009</v>
+        <v>0</v>
       </c>
       <c r="AA166">
-        <v>0.98000000000000009</v>
+        <v>0</v>
       </c>
       <c r="AB166">
-        <v>0.98000000000000009</v>
+        <v>0</v>
       </c>
       <c r="AC166">
-        <v>0.98000000000000009</v>
+        <v>0</v>
       </c>
       <c r="AD166">
-        <v>0.98000000000000009</v>
+        <v>0</v>
       </c>
       <c r="AE166">
-        <v>0.98000000000000009</v>
+        <v>0</v>
       </c>
       <c r="AF166">
-        <v>0.98000000000000009</v>
+        <v>0</v>
       </c>
       <c r="AG166">
-        <v>0.98000000000000009</v>
+        <v>0</v>
       </c>
     </row>
     <row r="167" spans="1:33" x14ac:dyDescent="0.3">
@@ -7304,7 +7554,7 @@
         <v>35</v>
       </c>
       <c r="B167" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C167" t="s">
         <v>24</v>
@@ -7319,85 +7569,85 @@
         <v>0</v>
       </c>
       <c r="G167">
-        <v>0</v>
+        <v>0.98000000000000009</v>
       </c>
       <c r="H167">
-        <v>3.5</v>
+        <v>0.98000000000000009</v>
       </c>
       <c r="I167">
-        <v>3.5</v>
+        <v>0.98000000000000009</v>
       </c>
       <c r="J167">
-        <v>3.5</v>
+        <v>0.98000000000000009</v>
       </c>
       <c r="K167">
-        <v>3.5</v>
+        <v>0.98000000000000009</v>
       </c>
       <c r="L167">
-        <v>3.5</v>
+        <v>0.98000000000000009</v>
       </c>
       <c r="M167">
-        <v>3.5</v>
+        <v>0.98000000000000009</v>
       </c>
       <c r="N167">
-        <v>7</v>
+        <v>0.98000000000000009</v>
       </c>
       <c r="O167">
-        <v>7</v>
+        <v>0.98000000000000009</v>
       </c>
       <c r="P167">
-        <v>7</v>
+        <v>0.98000000000000009</v>
       </c>
       <c r="Q167">
-        <v>7</v>
+        <v>0.98000000000000009</v>
       </c>
       <c r="R167">
-        <v>7</v>
+        <v>0.98000000000000009</v>
       </c>
       <c r="S167">
-        <v>7</v>
+        <v>0.98000000000000009</v>
       </c>
       <c r="T167">
-        <v>7</v>
+        <v>0.98000000000000009</v>
       </c>
       <c r="U167">
-        <v>7</v>
+        <v>0.98000000000000009</v>
       </c>
       <c r="V167">
-        <v>7</v>
+        <v>0.98000000000000009</v>
       </c>
       <c r="W167">
-        <v>7</v>
+        <v>0.98000000000000009</v>
       </c>
       <c r="X167">
-        <v>7</v>
+        <v>0.98000000000000009</v>
       </c>
       <c r="Y167">
-        <v>7</v>
+        <v>0.98000000000000009</v>
       </c>
       <c r="Z167">
-        <v>7</v>
+        <v>0.98000000000000009</v>
       </c>
       <c r="AA167">
-        <v>7</v>
+        <v>0.98000000000000009</v>
       </c>
       <c r="AB167">
-        <v>7</v>
+        <v>0.98000000000000009</v>
       </c>
       <c r="AC167">
-        <v>7</v>
+        <v>0.98000000000000009</v>
       </c>
       <c r="AD167">
-        <v>7</v>
+        <v>0.98000000000000009</v>
       </c>
       <c r="AE167">
-        <v>7</v>
+        <v>0.98000000000000009</v>
       </c>
       <c r="AF167">
-        <v>7</v>
+        <v>0.98000000000000009</v>
       </c>
       <c r="AG167">
-        <v>7</v>
+        <v>0.98000000000000009</v>
       </c>
     </row>
     <row r="168" spans="1:33" x14ac:dyDescent="0.3">
@@ -7405,16 +7655,16 @@
         <v>35</v>
       </c>
       <c r="B168" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C168" t="s">
         <v>24</v>
       </c>
       <c r="D168">
-        <v>1.89</v>
+        <v>0</v>
       </c>
       <c r="E168">
-        <v>1.89</v>
+        <v>0</v>
       </c>
       <c r="F168">
         <v>0</v>
@@ -7423,82 +7673,82 @@
         <v>0</v>
       </c>
       <c r="H168">
-        <v>0</v>
+        <v>3.5</v>
       </c>
       <c r="I168">
-        <v>0</v>
+        <v>3.5</v>
       </c>
       <c r="J168">
-        <v>0</v>
+        <v>3.5</v>
       </c>
       <c r="K168">
-        <v>0</v>
+        <v>3.5</v>
       </c>
       <c r="L168">
-        <v>0</v>
+        <v>3.5</v>
       </c>
       <c r="M168">
-        <v>0</v>
+        <v>3.5</v>
       </c>
       <c r="N168">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="O168">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="P168">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="Q168">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="R168">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="S168">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="T168">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="U168">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="V168">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="W168">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="X168">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="Y168">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="Z168">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AA168">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AB168">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AC168">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AD168">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AE168">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AF168">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AG168">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="169" spans="1:33" x14ac:dyDescent="0.3">
@@ -7506,7 +7756,7 @@
         <v>35</v>
       </c>
       <c r="B169" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C169" t="s">
         <v>24</v>
@@ -7607,16 +7857,16 @@
         <v>35</v>
       </c>
       <c r="B170" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C170" t="s">
         <v>24</v>
       </c>
       <c r="D170">
-        <v>0</v>
+        <v>1.89</v>
       </c>
       <c r="E170">
-        <v>1.26</v>
+        <v>1.89</v>
       </c>
       <c r="F170">
         <v>0</v>
@@ -7708,100 +7958,100 @@
         <v>35</v>
       </c>
       <c r="B171" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C171" t="s">
         <v>24</v>
       </c>
       <c r="D171">
-        <v>1.764</v>
+        <v>0</v>
       </c>
       <c r="E171">
-        <v>1.764</v>
+        <v>1.26</v>
       </c>
       <c r="F171">
-        <v>1.764</v>
+        <v>0</v>
       </c>
       <c r="G171">
-        <v>1.764</v>
+        <v>0</v>
       </c>
       <c r="H171">
-        <v>1.764</v>
+        <v>0</v>
       </c>
       <c r="I171">
-        <v>1.764</v>
+        <v>0</v>
       </c>
       <c r="J171">
-        <v>1.764</v>
+        <v>0</v>
       </c>
       <c r="K171">
-        <v>1.764</v>
+        <v>0</v>
       </c>
       <c r="L171">
-        <v>1.764</v>
+        <v>0</v>
       </c>
       <c r="M171">
-        <v>1.764</v>
+        <v>0</v>
       </c>
       <c r="N171">
-        <v>1.764</v>
+        <v>0</v>
       </c>
       <c r="O171">
-        <v>1.764</v>
+        <v>0</v>
       </c>
       <c r="P171">
-        <v>1.764</v>
+        <v>0</v>
       </c>
       <c r="Q171">
-        <v>1.764</v>
+        <v>0</v>
       </c>
       <c r="R171">
-        <v>1.764</v>
+        <v>0</v>
       </c>
       <c r="S171">
-        <v>1.764</v>
+        <v>0</v>
       </c>
       <c r="T171">
-        <v>1.764</v>
+        <v>0</v>
       </c>
       <c r="U171">
-        <v>1.764</v>
+        <v>0</v>
       </c>
       <c r="V171">
-        <v>1.764</v>
+        <v>0</v>
       </c>
       <c r="W171">
-        <v>1.764</v>
+        <v>0</v>
       </c>
       <c r="X171">
-        <v>1.764</v>
+        <v>0</v>
       </c>
       <c r="Y171">
-        <v>1.764</v>
+        <v>0</v>
       </c>
       <c r="Z171">
-        <v>1.764</v>
+        <v>0</v>
       </c>
       <c r="AA171">
-        <v>1.764</v>
+        <v>0</v>
       </c>
       <c r="AB171">
-        <v>1.764</v>
+        <v>0</v>
       </c>
       <c r="AC171">
-        <v>1.764</v>
+        <v>0</v>
       </c>
       <c r="AD171">
-        <v>1.764</v>
+        <v>0</v>
       </c>
       <c r="AE171">
-        <v>1.764</v>
+        <v>0</v>
       </c>
       <c r="AF171">
-        <v>1.764</v>
+        <v>0</v>
       </c>
       <c r="AG171">
-        <v>1.764</v>
+        <v>0</v>
       </c>
     </row>
     <row r="172" spans="1:33" x14ac:dyDescent="0.3">
@@ -7809,100 +8059,100 @@
         <v>35</v>
       </c>
       <c r="B172" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C172" t="s">
         <v>24</v>
       </c>
       <c r="D172">
-        <v>0</v>
+        <v>1.764</v>
       </c>
       <c r="E172">
-        <v>0</v>
+        <v>1.764</v>
       </c>
       <c r="F172">
-        <v>0</v>
+        <v>1.764</v>
       </c>
       <c r="G172">
-        <v>5.04</v>
+        <v>1.764</v>
       </c>
       <c r="H172">
-        <v>5.04</v>
+        <v>1.764</v>
       </c>
       <c r="I172">
-        <v>5.04</v>
+        <v>1.764</v>
       </c>
       <c r="J172">
-        <v>5.7960000000000003</v>
+        <v>1.764</v>
       </c>
       <c r="K172">
-        <v>5.7960000000000003</v>
+        <v>1.764</v>
       </c>
       <c r="L172">
-        <v>5.7960000000000003</v>
+        <v>1.764</v>
       </c>
       <c r="M172">
-        <v>5.7960000000000003</v>
+        <v>1.764</v>
       </c>
       <c r="N172">
-        <v>5.7960000000000003</v>
+        <v>1.764</v>
       </c>
       <c r="O172">
-        <v>5.7960000000000003</v>
+        <v>1.764</v>
       </c>
       <c r="P172">
-        <v>5.7960000000000003</v>
+        <v>1.764</v>
       </c>
       <c r="Q172">
-        <v>5.7960000000000003</v>
+        <v>1.764</v>
       </c>
       <c r="R172">
-        <v>5.7960000000000003</v>
+        <v>1.764</v>
       </c>
       <c r="S172">
-        <v>5.7960000000000003</v>
+        <v>1.764</v>
       </c>
       <c r="T172">
-        <v>5.7960000000000003</v>
+        <v>1.764</v>
       </c>
       <c r="U172">
-        <v>5.7960000000000003</v>
+        <v>1.764</v>
       </c>
       <c r="V172">
-        <v>5.7960000000000003</v>
+        <v>1.764</v>
       </c>
       <c r="W172">
-        <v>5.7960000000000003</v>
+        <v>1.764</v>
       </c>
       <c r="X172">
-        <v>5.7960000000000003</v>
+        <v>1.764</v>
       </c>
       <c r="Y172">
-        <v>5.7960000000000003</v>
+        <v>1.764</v>
       </c>
       <c r="Z172">
-        <v>5.7960000000000003</v>
+        <v>1.764</v>
       </c>
       <c r="AA172">
-        <v>5.7960000000000003</v>
+        <v>1.764</v>
       </c>
       <c r="AB172">
-        <v>5.7960000000000003</v>
+        <v>1.764</v>
       </c>
       <c r="AC172">
-        <v>5.7960000000000003</v>
+        <v>1.764</v>
       </c>
       <c r="AD172">
-        <v>5.7960000000000003</v>
+        <v>1.764</v>
       </c>
       <c r="AE172">
-        <v>5.7960000000000003</v>
+        <v>1.764</v>
       </c>
       <c r="AF172">
-        <v>5.7960000000000003</v>
+        <v>1.764</v>
       </c>
       <c r="AG172">
-        <v>5.7960000000000003</v>
+        <v>1.764</v>
       </c>
     </row>
     <row r="173" spans="1:33" x14ac:dyDescent="0.3">
@@ -7910,7 +8160,7 @@
         <v>35</v>
       </c>
       <c r="B173" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C173" t="s">
         <v>24</v>
@@ -7925,85 +8175,85 @@
         <v>0</v>
       </c>
       <c r="G173">
-        <v>0</v>
+        <v>5.04</v>
       </c>
       <c r="H173">
-        <v>0</v>
+        <v>5.04</v>
       </c>
       <c r="I173">
-        <v>0</v>
+        <v>5.04</v>
       </c>
       <c r="J173">
-        <v>0</v>
+        <v>5.7960000000000003</v>
       </c>
       <c r="K173">
-        <v>0</v>
+        <v>5.7960000000000003</v>
       </c>
       <c r="L173">
-        <v>0</v>
+        <v>5.7960000000000003</v>
       </c>
       <c r="M173">
-        <v>0</v>
+        <v>5.7960000000000003</v>
       </c>
       <c r="N173">
-        <v>0</v>
+        <v>5.7960000000000003</v>
       </c>
       <c r="O173">
-        <v>0</v>
+        <v>5.7960000000000003</v>
       </c>
       <c r="P173">
-        <v>0</v>
+        <v>5.7960000000000003</v>
       </c>
       <c r="Q173">
-        <v>0</v>
+        <v>5.7960000000000003</v>
       </c>
       <c r="R173">
-        <v>0</v>
+        <v>5.7960000000000003</v>
       </c>
       <c r="S173">
-        <v>0</v>
+        <v>5.7960000000000003</v>
       </c>
       <c r="T173">
-        <v>0</v>
+        <v>5.7960000000000003</v>
       </c>
       <c r="U173">
-        <v>0</v>
+        <v>5.7960000000000003</v>
       </c>
       <c r="V173">
-        <v>0</v>
+        <v>5.7960000000000003</v>
       </c>
       <c r="W173">
-        <v>0</v>
+        <v>5.7960000000000003</v>
       </c>
       <c r="X173">
-        <v>0</v>
+        <v>5.7960000000000003</v>
       </c>
       <c r="Y173">
-        <v>0</v>
+        <v>5.7960000000000003</v>
       </c>
       <c r="Z173">
-        <v>0</v>
+        <v>5.7960000000000003</v>
       </c>
       <c r="AA173">
-        <v>0</v>
+        <v>5.7960000000000003</v>
       </c>
       <c r="AB173">
-        <v>0</v>
+        <v>5.7960000000000003</v>
       </c>
       <c r="AC173">
-        <v>0</v>
+        <v>5.7960000000000003</v>
       </c>
       <c r="AD173">
-        <v>0</v>
+        <v>5.7960000000000003</v>
       </c>
       <c r="AE173">
-        <v>0</v>
+        <v>5.7960000000000003</v>
       </c>
       <c r="AF173">
-        <v>0</v>
+        <v>5.7960000000000003</v>
       </c>
       <c r="AG173">
-        <v>0</v>
+        <v>5.7960000000000003</v>
       </c>
     </row>
     <row r="174" spans="1:33" x14ac:dyDescent="0.3">
@@ -8011,7 +8261,7 @@
         <v>35</v>
       </c>
       <c r="B174" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C174" t="s">
         <v>24</v>
@@ -8020,13 +8270,13 @@
         <v>0</v>
       </c>
       <c r="E174">
-        <v>11.25</v>
+        <v>0</v>
       </c>
       <c r="F174">
-        <v>9.75</v>
+        <v>0</v>
       </c>
       <c r="G174">
-        <v>7.5</v>
+        <v>0</v>
       </c>
       <c r="H174">
         <v>0</v>
@@ -8112,13 +8362,13 @@
         <v>35</v>
       </c>
       <c r="B175" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C175" t="s">
         <v>24</v>
       </c>
       <c r="D175">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="E175">
         <v>11.25</v>
@@ -8213,22 +8463,22 @@
         <v>35</v>
       </c>
       <c r="B176" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C176" t="s">
         <v>24</v>
       </c>
       <c r="D176">
-        <v>22.400000000000002</v>
+        <v>12</v>
       </c>
       <c r="E176">
-        <v>21</v>
+        <v>11.25</v>
       </c>
       <c r="F176">
-        <v>18.2</v>
+        <v>9.75</v>
       </c>
       <c r="G176">
-        <v>14</v>
+        <v>7.5</v>
       </c>
       <c r="H176">
         <v>0</v>
@@ -8314,22 +8564,22 @@
         <v>35</v>
       </c>
       <c r="B177" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C177" t="s">
         <v>24</v>
       </c>
       <c r="D177">
-        <v>5.6000000000000005</v>
+        <v>22.400000000000002</v>
       </c>
       <c r="E177">
-        <v>5.25</v>
+        <v>21</v>
       </c>
       <c r="F177">
-        <v>4.55</v>
+        <v>18.2</v>
       </c>
       <c r="G177">
-        <v>3.5</v>
+        <v>14</v>
       </c>
       <c r="H177">
         <v>0</v>
@@ -8415,7 +8665,7 @@
         <v>35</v>
       </c>
       <c r="B178" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C178" t="s">
         <v>24</v>
@@ -8516,22 +8766,22 @@
         <v>35</v>
       </c>
       <c r="B179" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C179" t="s">
         <v>24</v>
       </c>
       <c r="D179">
-        <v>48</v>
+        <v>5.6000000000000005</v>
       </c>
       <c r="E179">
-        <v>45</v>
+        <v>5.25</v>
       </c>
       <c r="F179">
-        <v>39</v>
+        <v>4.55</v>
       </c>
       <c r="G179">
-        <v>30</v>
+        <v>3.5</v>
       </c>
       <c r="H179">
         <v>0</v>
@@ -8617,22 +8867,22 @@
         <v>35</v>
       </c>
       <c r="B180" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C180" t="s">
         <v>24</v>
       </c>
       <c r="D180">
-        <v>4.8000000000000007</v>
+        <v>48</v>
       </c>
       <c r="E180">
-        <v>4.5</v>
+        <v>45</v>
       </c>
       <c r="F180">
-        <v>3.9000000000000004</v>
+        <v>39</v>
       </c>
       <c r="G180">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="H180">
         <v>0</v>
@@ -8718,22 +8968,22 @@
         <v>35</v>
       </c>
       <c r="B181" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C181" t="s">
         <v>24</v>
       </c>
       <c r="D181">
-        <v>0</v>
+        <v>4.8000000000000007</v>
       </c>
       <c r="E181">
-        <v>0</v>
+        <v>4.5</v>
       </c>
       <c r="F181">
-        <v>0</v>
+        <v>3.9000000000000004</v>
       </c>
       <c r="G181">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H181">
         <v>0</v>
@@ -8748,7 +8998,7 @@
         <v>0</v>
       </c>
       <c r="L181">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="M181">
         <v>0</v>
@@ -8763,7 +9013,7 @@
         <v>0</v>
       </c>
       <c r="Q181">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="R181">
         <v>0</v>
@@ -8778,7 +9028,7 @@
         <v>0</v>
       </c>
       <c r="V181">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="W181">
         <v>0</v>
@@ -8793,7 +9043,7 @@
         <v>0</v>
       </c>
       <c r="AA181">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="AB181">
         <v>0</v>
@@ -8808,7 +9058,7 @@
         <v>0</v>
       </c>
       <c r="AF181">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="AG181">
         <v>0</v>
@@ -8819,7 +9069,7 @@
         <v>35</v>
       </c>
       <c r="B182" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C182" t="s">
         <v>24</v>
@@ -8834,85 +9084,85 @@
         <v>0</v>
       </c>
       <c r="G182">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H182">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I182">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J182">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="K182">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="L182">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M182">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="N182">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="O182">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="P182">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="Q182">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="R182">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="S182">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="T182">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="U182">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="V182">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="W182">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="X182">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="Y182">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="Z182">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AA182">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AB182">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AC182">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AD182">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AE182">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AF182">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AG182">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="183" spans="1:33" x14ac:dyDescent="0.3">
@@ -8920,7 +9170,7 @@
         <v>35</v>
       </c>
       <c r="B183" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C183" t="s">
         <v>24</v>
@@ -8938,385 +9188,284 @@
         <v>0</v>
       </c>
       <c r="H183">
+        <v>4</v>
+      </c>
+      <c r="I183">
+        <v>4</v>
+      </c>
+      <c r="J183">
+        <v>4</v>
+      </c>
+      <c r="K183">
+        <v>4</v>
+      </c>
+      <c r="L183">
+        <v>4</v>
+      </c>
+      <c r="M183">
+        <v>4</v>
+      </c>
+      <c r="N183">
+        <v>4</v>
+      </c>
+      <c r="O183">
+        <v>4</v>
+      </c>
+      <c r="P183">
+        <v>4</v>
+      </c>
+      <c r="Q183">
+        <v>4</v>
+      </c>
+      <c r="R183">
+        <v>4</v>
+      </c>
+      <c r="S183">
+        <v>4</v>
+      </c>
+      <c r="T183">
+        <v>4</v>
+      </c>
+      <c r="U183">
+        <v>4</v>
+      </c>
+      <c r="V183">
+        <v>4</v>
+      </c>
+      <c r="W183">
+        <v>4</v>
+      </c>
+      <c r="X183">
+        <v>4</v>
+      </c>
+      <c r="Y183">
+        <v>4</v>
+      </c>
+      <c r="Z183">
+        <v>4</v>
+      </c>
+      <c r="AA183">
+        <v>4</v>
+      </c>
+      <c r="AB183">
+        <v>4</v>
+      </c>
+      <c r="AC183">
+        <v>4</v>
+      </c>
+      <c r="AD183">
+        <v>4</v>
+      </c>
+      <c r="AE183">
+        <v>4</v>
+      </c>
+      <c r="AF183">
+        <v>4</v>
+      </c>
+      <c r="AG183">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="184" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="A184" t="s">
+        <v>35</v>
+      </c>
+      <c r="B184" t="s">
+        <v>111</v>
+      </c>
+      <c r="C184" t="s">
+        <v>24</v>
+      </c>
+      <c r="D184">
+        <v>0</v>
+      </c>
+      <c r="E184">
+        <v>0</v>
+      </c>
+      <c r="F184">
+        <v>0</v>
+      </c>
+      <c r="G184">
+        <v>0</v>
+      </c>
+      <c r="H184">
         <v>3</v>
       </c>
-      <c r="I183">
+      <c r="I184">
         <v>3</v>
       </c>
-      <c r="J183">
+      <c r="J184">
         <v>3</v>
       </c>
-      <c r="K183">
+      <c r="K184">
         <v>3</v>
       </c>
-      <c r="L183">
+      <c r="L184">
         <v>3</v>
       </c>
-      <c r="M183">
+      <c r="M184">
         <v>3</v>
       </c>
-      <c r="N183">
+      <c r="N184">
         <v>3</v>
       </c>
-      <c r="O183">
+      <c r="O184">
         <v>3</v>
       </c>
-      <c r="P183">
+      <c r="P184">
         <v>3</v>
       </c>
-      <c r="Q183">
+      <c r="Q184">
         <v>3</v>
       </c>
-      <c r="R183">
+      <c r="R184">
         <v>3</v>
       </c>
-      <c r="S183">
+      <c r="S184">
         <v>3</v>
       </c>
-      <c r="T183">
+      <c r="T184">
         <v>3</v>
       </c>
-      <c r="U183">
+      <c r="U184">
         <v>3</v>
       </c>
-      <c r="V183">
+      <c r="V184">
         <v>3</v>
       </c>
-      <c r="W183">
+      <c r="W184">
         <v>3</v>
       </c>
-      <c r="X183">
+      <c r="X184">
         <v>3</v>
       </c>
-      <c r="Y183">
+      <c r="Y184">
         <v>3</v>
       </c>
-      <c r="Z183">
+      <c r="Z184">
         <v>3</v>
       </c>
-      <c r="AA183">
+      <c r="AA184">
         <v>3</v>
       </c>
-      <c r="AB183">
+      <c r="AB184">
         <v>3</v>
       </c>
-      <c r="AC183">
+      <c r="AC184">
         <v>3</v>
       </c>
-      <c r="AD183">
+      <c r="AD184">
         <v>3</v>
       </c>
-      <c r="AE183">
+      <c r="AE184">
         <v>3</v>
       </c>
-      <c r="AF183">
+      <c r="AF184">
         <v>3</v>
       </c>
-      <c r="AG183">
+      <c r="AG184">
         <v>3</v>
       </c>
     </row>
-    <row r="184" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A184" s="1" t="s">
+    <row r="186" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="A186" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B184" t="s">
+      <c r="B186" t="s">
         <v>88</v>
-      </c>
-      <c r="C184" t="s">
-        <v>112</v>
-      </c>
-      <c r="D184">
-        <v>0</v>
-      </c>
-      <c r="E184">
-        <v>0</v>
-      </c>
-      <c r="F184">
-        <v>0</v>
-      </c>
-      <c r="G184">
-        <v>94.5</v>
-      </c>
-      <c r="H184">
-        <v>118.125</v>
-      </c>
-      <c r="I184">
-        <v>141.75</v>
-      </c>
-      <c r="J184">
-        <v>165.375</v>
-      </c>
-      <c r="K184">
-        <v>189</v>
-      </c>
-      <c r="L184">
-        <v>212.625</v>
-      </c>
-      <c r="M184">
-        <v>236.25</v>
-      </c>
-      <c r="N184">
-        <v>259.875</v>
-      </c>
-      <c r="O184">
-        <v>307.125</v>
-      </c>
-      <c r="P184">
-        <v>354.375</v>
-      </c>
-      <c r="Q184">
-        <v>401.625</v>
-      </c>
-      <c r="R184">
-        <v>448.875</v>
-      </c>
-      <c r="S184">
-        <v>496.125</v>
-      </c>
-      <c r="T184">
-        <v>543.375</v>
-      </c>
-      <c r="U184">
-        <v>519.75</v>
-      </c>
-      <c r="V184">
-        <v>496.125</v>
-      </c>
-      <c r="W184">
-        <v>472.5</v>
-      </c>
-      <c r="X184">
-        <v>448.875</v>
-      </c>
-      <c r="Y184">
-        <v>425.25</v>
-      </c>
-      <c r="Z184">
-        <v>401.625</v>
-      </c>
-      <c r="AA184">
-        <v>363.82500000000005</v>
-      </c>
-      <c r="AB184">
-        <v>326.02500000000003</v>
-      </c>
-      <c r="AC184">
-        <v>288.22500000000002</v>
-      </c>
-      <c r="AD184">
-        <v>250.42500000000004</v>
-      </c>
-      <c r="AE184">
-        <v>226.80000000000004</v>
-      </c>
-      <c r="AF184">
-        <v>203.17500000000004</v>
-      </c>
-      <c r="AG184">
-        <v>179.55000000000004</v>
-      </c>
-    </row>
-    <row r="185" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A185" t="s">
-        <v>119</v>
-      </c>
-      <c r="B185" t="s">
-        <v>89</v>
-      </c>
-      <c r="C185" t="s">
-        <v>112</v>
-      </c>
-      <c r="D185">
-        <v>0</v>
-      </c>
-      <c r="E185">
-        <v>0</v>
-      </c>
-      <c r="F185">
-        <v>0</v>
-      </c>
-      <c r="G185">
-        <v>0</v>
-      </c>
-      <c r="H185">
-        <v>366.13866314846564</v>
-      </c>
-      <c r="I185">
-        <v>549.20799472269846</v>
-      </c>
-      <c r="J185">
-        <v>549.20799472269846</v>
-      </c>
-      <c r="K185">
-        <v>549.20799472269846</v>
-      </c>
-      <c r="L185">
-        <v>732.27732629693128</v>
-      </c>
-      <c r="M185">
-        <v>732.27732629693128</v>
-      </c>
-      <c r="N185">
-        <v>732.27732629693128</v>
-      </c>
-      <c r="O185">
-        <v>732.27732629693128</v>
-      </c>
-      <c r="P185">
-        <v>866.55445126487166</v>
-      </c>
-      <c r="Q185">
-        <v>866.55445126487166</v>
-      </c>
-      <c r="R185">
-        <v>1000.8315762328122</v>
-      </c>
-      <c r="S185">
-        <v>1002.1065744316124</v>
-      </c>
-      <c r="T185">
-        <v>1003.3815726304125</v>
-      </c>
-      <c r="U185">
-        <v>1004.6565708292128</v>
-      </c>
-      <c r="V185">
-        <v>1005.9315690280127</v>
-      </c>
-      <c r="W185">
-        <v>1007.206567226813</v>
-      </c>
-      <c r="X185">
-        <v>1008.4815654256133</v>
-      </c>
-      <c r="Y185">
-        <v>1009.7565636244134</v>
-      </c>
-      <c r="Z185">
-        <v>1011.0315618232135</v>
-      </c>
-      <c r="AA185">
-        <v>1012.3065600220139</v>
-      </c>
-      <c r="AB185">
-        <v>1013.581558220814</v>
-      </c>
-      <c r="AC185">
-        <v>1014.8565564196142</v>
-      </c>
-      <c r="AD185">
-        <v>1016.1315546184143</v>
-      </c>
-      <c r="AE185">
-        <v>1017.4065528172146</v>
-      </c>
-      <c r="AF185">
-        <v>1018.6815510160146</v>
-      </c>
-      <c r="AG185">
-        <v>1019.9565492148149</v>
-      </c>
-    </row>
-    <row r="186" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A186" t="s">
-        <v>119</v>
-      </c>
-      <c r="B186" t="s">
-        <v>90</v>
       </c>
       <c r="C186" t="s">
         <v>112</v>
       </c>
       <c r="D186">
-        <v>10080</v>
+        <v>0</v>
       </c>
       <c r="E186">
-        <v>9450</v>
+        <v>0</v>
       </c>
       <c r="F186">
-        <v>8190</v>
+        <v>0</v>
       </c>
       <c r="G186">
-        <v>6300</v>
+        <v>94.5</v>
       </c>
       <c r="H186">
-        <v>0</v>
+        <v>118.125</v>
       </c>
       <c r="I186">
-        <v>0</v>
+        <v>141.75</v>
       </c>
       <c r="J186">
-        <v>0</v>
+        <v>165.375</v>
       </c>
       <c r="K186">
-        <v>0</v>
+        <v>189</v>
       </c>
       <c r="L186">
-        <v>0</v>
+        <v>212.625</v>
       </c>
       <c r="M186">
-        <v>0</v>
+        <v>236.25</v>
       </c>
       <c r="N186">
-        <v>0</v>
+        <v>259.875</v>
       </c>
       <c r="O186">
-        <v>0</v>
+        <v>307.125</v>
       </c>
       <c r="P186">
-        <v>0</v>
+        <v>354.375</v>
       </c>
       <c r="Q186">
-        <v>0</v>
+        <v>401.625</v>
       </c>
       <c r="R186">
-        <v>0</v>
+        <v>448.875</v>
       </c>
       <c r="S186">
-        <v>0</v>
+        <v>496.125</v>
       </c>
       <c r="T186">
-        <v>0</v>
+        <v>543.375</v>
       </c>
       <c r="U186">
-        <v>0</v>
+        <v>519.75</v>
       </c>
       <c r="V186">
-        <v>0</v>
+        <v>496.125</v>
       </c>
       <c r="W186">
-        <v>0</v>
+        <v>472.5</v>
       </c>
       <c r="X186">
-        <v>0</v>
+        <v>448.875</v>
       </c>
       <c r="Y186">
-        <v>0</v>
+        <v>425.25</v>
       </c>
       <c r="Z186">
-        <v>0</v>
+        <v>401.625</v>
       </c>
       <c r="AA186">
-        <v>0</v>
+        <v>363.82500000000005</v>
       </c>
       <c r="AB186">
-        <v>0</v>
+        <v>326.02500000000003</v>
       </c>
       <c r="AC186">
-        <v>0</v>
+        <v>288.22500000000002</v>
       </c>
       <c r="AD186">
-        <v>0</v>
+        <v>250.42500000000004</v>
       </c>
       <c r="AE186">
-        <v>0</v>
+        <v>226.80000000000004</v>
       </c>
       <c r="AF186">
-        <v>0</v>
+        <v>203.17500000000004</v>
       </c>
       <c r="AG186">
-        <v>0</v>
+        <v>179.55000000000004</v>
       </c>
     </row>
     <row r="187" spans="1:33" x14ac:dyDescent="0.3">
@@ -9324,7 +9473,7 @@
         <v>119</v>
       </c>
       <c r="B187" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C187" t="s">
         <v>112</v>
@@ -9342,81 +9491,283 @@
         <v>0</v>
       </c>
       <c r="H187">
+        <v>366.13866314846564</v>
+      </c>
+      <c r="I187">
+        <v>549.20799472269846</v>
+      </c>
+      <c r="J187">
+        <v>549.20799472269846</v>
+      </c>
+      <c r="K187">
+        <v>549.20799472269846</v>
+      </c>
+      <c r="L187">
+        <v>732.27732629693128</v>
+      </c>
+      <c r="M187">
+        <v>732.27732629693128</v>
+      </c>
+      <c r="N187">
+        <v>732.27732629693128</v>
+      </c>
+      <c r="O187">
+        <v>732.27732629693128</v>
+      </c>
+      <c r="P187">
+        <v>866.55445126487166</v>
+      </c>
+      <c r="Q187">
+        <v>866.55445126487166</v>
+      </c>
+      <c r="R187">
+        <v>1000.8315762328122</v>
+      </c>
+      <c r="S187">
+        <v>1002.1065744316124</v>
+      </c>
+      <c r="T187">
+        <v>1003.3815726304125</v>
+      </c>
+      <c r="U187">
+        <v>1004.6565708292128</v>
+      </c>
+      <c r="V187">
+        <v>1005.9315690280127</v>
+      </c>
+      <c r="W187">
+        <v>1007.206567226813</v>
+      </c>
+      <c r="X187">
+        <v>1008.4815654256133</v>
+      </c>
+      <c r="Y187">
+        <v>1009.7565636244134</v>
+      </c>
+      <c r="Z187">
+        <v>1011.0315618232135</v>
+      </c>
+      <c r="AA187">
+        <v>1012.3065600220139</v>
+      </c>
+      <c r="AB187">
+        <v>1013.581558220814</v>
+      </c>
+      <c r="AC187">
+        <v>1014.8565564196142</v>
+      </c>
+      <c r="AD187">
+        <v>1016.1315546184143</v>
+      </c>
+      <c r="AE187">
+        <v>1017.4065528172146</v>
+      </c>
+      <c r="AF187">
+        <v>1018.6815510160146</v>
+      </c>
+      <c r="AG187">
+        <v>1019.9565492148149</v>
+      </c>
+    </row>
+    <row r="188" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="A188" t="s">
+        <v>119</v>
+      </c>
+      <c r="B188" t="s">
+        <v>90</v>
+      </c>
+      <c r="C188" t="s">
+        <v>112</v>
+      </c>
+      <c r="D188">
+        <v>10080</v>
+      </c>
+      <c r="E188">
+        <v>9450</v>
+      </c>
+      <c r="F188">
+        <v>8190</v>
+      </c>
+      <c r="G188">
+        <v>6300</v>
+      </c>
+      <c r="H188">
+        <v>0</v>
+      </c>
+      <c r="I188">
+        <v>0</v>
+      </c>
+      <c r="J188">
+        <v>0</v>
+      </c>
+      <c r="K188">
+        <v>0</v>
+      </c>
+      <c r="L188">
+        <v>0</v>
+      </c>
+      <c r="M188">
+        <v>0</v>
+      </c>
+      <c r="N188">
+        <v>0</v>
+      </c>
+      <c r="O188">
+        <v>0</v>
+      </c>
+      <c r="P188">
+        <v>0</v>
+      </c>
+      <c r="Q188">
+        <v>0</v>
+      </c>
+      <c r="R188">
+        <v>0</v>
+      </c>
+      <c r="S188">
+        <v>0</v>
+      </c>
+      <c r="T188">
+        <v>0</v>
+      </c>
+      <c r="U188">
+        <v>0</v>
+      </c>
+      <c r="V188">
+        <v>0</v>
+      </c>
+      <c r="W188">
+        <v>0</v>
+      </c>
+      <c r="X188">
+        <v>0</v>
+      </c>
+      <c r="Y188">
+        <v>0</v>
+      </c>
+      <c r="Z188">
+        <v>0</v>
+      </c>
+      <c r="AA188">
+        <v>0</v>
+      </c>
+      <c r="AB188">
+        <v>0</v>
+      </c>
+      <c r="AC188">
+        <v>0</v>
+      </c>
+      <c r="AD188">
+        <v>0</v>
+      </c>
+      <c r="AE188">
+        <v>0</v>
+      </c>
+      <c r="AF188">
+        <v>0</v>
+      </c>
+      <c r="AG188">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="189" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="A189" t="s">
+        <v>119</v>
+      </c>
+      <c r="B189" t="s">
+        <v>91</v>
+      </c>
+      <c r="C189" t="s">
+        <v>112</v>
+      </c>
+      <c r="D189">
+        <v>0</v>
+      </c>
+      <c r="E189">
+        <v>0</v>
+      </c>
+      <c r="F189">
+        <v>0</v>
+      </c>
+      <c r="G189">
+        <v>0</v>
+      </c>
+      <c r="H189">
         <v>168</v>
       </c>
-      <c r="I187">
+      <c r="I189">
         <v>168</v>
       </c>
-      <c r="J187">
+      <c r="J189">
         <v>168</v>
       </c>
-      <c r="K187">
+      <c r="K189">
         <v>168</v>
       </c>
-      <c r="L187">
+      <c r="L189">
         <v>168</v>
       </c>
-      <c r="M187">
+      <c r="M189">
         <v>168</v>
       </c>
-      <c r="N187">
+      <c r="N189">
         <v>168</v>
       </c>
-      <c r="O187">
+      <c r="O189">
         <v>168</v>
       </c>
-      <c r="P187">
+      <c r="P189">
         <v>168</v>
       </c>
-      <c r="Q187">
+      <c r="Q189">
         <v>168</v>
       </c>
-      <c r="R187">
+      <c r="R189">
         <v>168</v>
       </c>
-      <c r="S187">
+      <c r="S189">
         <v>168</v>
       </c>
-      <c r="T187">
+      <c r="T189">
         <v>168</v>
       </c>
-      <c r="U187">
+      <c r="U189">
         <v>168</v>
       </c>
-      <c r="V187">
+      <c r="V189">
         <v>168</v>
       </c>
-      <c r="W187">
+      <c r="W189">
         <v>168</v>
       </c>
-      <c r="X187">
+      <c r="X189">
         <v>168</v>
       </c>
-      <c r="Y187">
+      <c r="Y189">
         <v>168</v>
       </c>
-      <c r="Z187">
+      <c r="Z189">
         <v>168</v>
       </c>
-      <c r="AA187">
+      <c r="AA189">
         <v>168</v>
       </c>
-      <c r="AB187">
+      <c r="AB189">
         <v>168</v>
       </c>
-      <c r="AC187">
+      <c r="AC189">
         <v>168</v>
       </c>
-      <c r="AD187">
+      <c r="AD189">
         <v>168</v>
       </c>
-      <c r="AE187">
+      <c r="AE189">
         <v>168</v>
       </c>
-      <c r="AF187">
+      <c r="AF189">
         <v>168</v>
       </c>
-      <c r="AG187">
+      <c r="AG189">
         <v>168</v>
       </c>
     </row>

</xml_diff>